<commit_message>
Updated with new offer
</commit_message>
<xml_diff>
--- a/electricity_rates_2026/output/1mc/energy_cost_comparison_2026_1mc.xlsx
+++ b/electricity_rates_2026/output/1mc/energy_cost_comparison_2026_1mc.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,170 +451,190 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bord Gáis - Smart EV Bonus</t>
+          <t>Yuno Energy - D Smart Bonus + 6%</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1443.73</v>
+        <v>1402.35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pinergy - Nighttime</t>
+          <t>Energia Offer</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1579.96</v>
+        <v>1441.77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Flogas - Fixed</t>
+          <t>Bord Gáis - Smart EV Bonus</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1588.46</v>
+        <v>1443.73</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Community Power - Smart SST_DG1_CP_23</t>
+          <t>Pinergy - Nighttime</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1604.32</v>
+        <v>1579.96</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Yuno Energy - Dual Smart</t>
+          <t>Flogas - Fixed</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1624.34</v>
+        <v>1588.46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Electric Ireland - Dual SST</t>
+          <t>Community Power - Smart SST_DG1_CP_23</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1670.12</v>
+        <v>1604.32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Bord Gáis - Smart All Day</t>
+          <t>Yuno Energy - Dual Smart</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1702.32</v>
+        <v>1624.34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Flogas - Smart 24hr</t>
+          <t>Electric Ireland - Dual SST</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1733.09</v>
+        <v>1670.12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Flogas - Smart EV</t>
+          <t>Bord Gáis - Smart All Day</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1766.75</v>
+        <v>1702.32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Energia - Smart MCC12</t>
+          <t>Flogas - Smart 24hr</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1779.43</v>
+        <v>1733.09</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>SSEAirtricity - Smart EVMax</t>
+          <t>Flogas - Smart EV</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1816.23</v>
+        <v>1766.75</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Yuno Energy - Day/Night Variable</t>
+          <t>Energia - Smart MCC12</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1831.29</v>
+        <v>1779.43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Bord Gáis - Smart Standard</t>
+          <t>SSEAirtricity - Smart EVMax</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1839.56</v>
+        <v>1816.23</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Energia - EV Smart Drive</t>
+          <t>Yuno Energy - Day/Night Variable</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1886.87</v>
+        <v>1831.29</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Electric Ireland - Nightboost</t>
+          <t>Bord Gáis - Smart Standard</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1926.44</v>
+        <v>1839.56</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Energia - EV</t>
+          <t>Energia - EV Smart Drive</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1930.53</v>
+        <v>1886.87</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>Electric Ireland - Nightboost</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1926.44</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Energia - EV</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1930.53</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>Yuno Energy - EV Variable</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B22" t="n">
         <v>1957.67</v>
       </c>
     </row>

</xml_diff>